<commit_message>
V3.2.6(gzwcm): Implement gzwcm_auto tools (info/slc/sum) with 4-button UI layout
- Renamed autoslc -> slc, autosum -> sum
- Abstracted VERSION and BATCH as module variables
- Restructured UI: 4 buttons in one line under 'gzwcm_auto tools' header
- Implemented info: match employee data by emp_nm/emp_id, enrich from emp.xlsx
- Implemented slc: keep default columns + dict.xlsx columns with rename mapping
- Implemented sum: filter by emp_nm from emp.xlsx, sum by emp_id, group by grp
- Fixed emp_id formatting: 8-digit string with leading zeros preserved
- Added EMP_NAME_COLUMN_NAMES, EMP_ID_COLUMN_NAMES to constants
- Pre-format Excel columns as text to prevent emp_id data corruption
- Sum results: total on top, then grp_sum followed by employees, sorted by grp + value desc
- Updated help.html with concise gzwcm tools documentation
- Enhanced main file docstring with architecture and feature details
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projs\Peel Potato\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF77111-CE45-4D67-A026-1F08629531F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4422A05-49F2-4F73-A003-95DF08785D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>old</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -173,187 +173,6 @@
   <si>
     <t>时点存款</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>管户连接客户连接时时点存款</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>管户连接客户年初时点存款</t>
-  </si>
-  <si>
-    <t>管户连接客户较连接时时点存款新增</t>
-  </si>
-  <si>
-    <t>管户连接客户较年初时点存款新增</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM月日均负增长金额</t>
-  </si>
-  <si>
-    <t>较年初AUM月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM月日均负增长金额</t>
-  </si>
-  <si>
-    <t>较连接时AUM月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM月日均负增长金额</t>
-  </si>
-  <si>
-    <t>连接时较年初AUM月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较年初AUM年日均负增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时AUM年日均负增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初AUM年日均负增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款月日均负增长金额</t>
-  </si>
-  <si>
-    <t>较年初存款月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款月日均负增长金额</t>
-  </si>
-  <si>
-    <t>较连接时存款月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款月日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款月日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款月日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款月日均负增长金额</t>
-  </si>
-  <si>
-    <t>连接时较年初存款月日均负增长金额占比</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较年初存款年日均负增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接较连接时存款年日均负增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款年日均正增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款年日均负增长客户数</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款年日均正增长金额</t>
-  </si>
-  <si>
-    <t>管户连接时较年初存款年日均负增长金额</t>
-  </si>
-  <si>
-    <t>直营管户连接年日均增量产能_当日</t>
-  </si>
-  <si>
-    <t>直营管户连接年日均增量产能_年累计</t>
   </si>
   <si>
     <t>当月晋升移交客户数(管户)</t>
@@ -368,6 +187,33 @@
   </si>
   <si>
     <t>当月晋升移交数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+  </si>
+  <si>
+    <t>时点AUM值_保险</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时点AUM值_保险趸缴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时点保险AUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时点保险趸缴AUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时点AUM值_保险期缴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时点保险期缴AUM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -418,10 +264,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -703,16 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -925,316 +774,45 @@
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B38" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>46</v>
+      <c r="A40" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>47</v>
+      <c r="A41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>48</v>
+      <c r="A42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>